<commit_message>
fixed problem with premise-generated market mix having no 'product' field and value when writing to bw database
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-biogas.xlsx
+++ b/premise/data/additional_inventories/lci-biogas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/GitHub/premise/premise/data/additional_inventories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C7904B8-7C30-B545-AABD-E7C528277CE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D6A4F86-13C1-3845-8416-3508BA4018C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="34720" yWindow="160" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="157">
   <si>
     <t>Activity</t>
   </si>
@@ -320,12 +320,6 @@
   </si>
   <si>
     <t>market for natural gas service station</t>
-  </si>
-  <si>
-    <t>Energy, gross calorific value, in biomass</t>
-  </si>
-  <si>
-    <t>natural resource::biotic</t>
   </si>
   <si>
     <t>heat and power co-generation, biogas, gas engine</t>
@@ -893,10 +887,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N108"/>
+  <dimension ref="A1:N107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="L91" sqref="L91"/>
+    <sheetView tabSelected="1" topLeftCell="A102" workbookViewId="0">
+      <selection activeCell="A127" sqref="A127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -923,10 +917,10 @@
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="M3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
@@ -937,7 +931,7 @@
         <v>58</v>
       </c>
       <c r="M4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
@@ -948,7 +942,7 @@
         <v>1</v>
       </c>
       <c r="M5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
@@ -956,7 +950,7 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
@@ -964,7 +958,7 @@
         <v>79</v>
       </c>
       <c r="B7" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
@@ -975,7 +969,7 @@
         <v>85</v>
       </c>
       <c r="M8" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
@@ -986,7 +980,7 @@
         <v>81</v>
       </c>
       <c r="M9" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
@@ -997,7 +991,7 @@
         <v>52</v>
       </c>
       <c r="M10" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="16" x14ac:dyDescent="0.2">
@@ -1005,7 +999,7 @@
         <v>8</v>
       </c>
       <c r="M11" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
@@ -1028,25 +1022,25 @@
         <v>13</v>
       </c>
       <c r="G12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H12" t="s">
+        <v>104</v>
+      </c>
+      <c r="I12" t="s">
+        <v>156</v>
+      </c>
+      <c r="J12" t="s">
         <v>105</v>
-      </c>
-      <c r="H12" t="s">
-        <v>106</v>
-      </c>
-      <c r="I12" t="s">
-        <v>158</v>
-      </c>
-      <c r="J12" t="s">
-        <v>107</v>
       </c>
       <c r="K12" t="s">
         <v>1</v>
       </c>
       <c r="L12" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="M12" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="N12" t="s">
         <v>5</v>
@@ -1054,7 +1048,7 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -1066,7 +1060,7 @@
         <v>52</v>
       </c>
       <c r="E13" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F13" t="s">
         <v>30</v>
@@ -1075,18 +1069,18 @@
         <v>100</v>
       </c>
       <c r="K13" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="L13" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="N13" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B14">
         <v>4.6073299999999991E-12</v>
@@ -1095,7 +1089,7 @@
         <v>7</v>
       </c>
       <c r="E14" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F14" t="s">
         <v>19</v>
@@ -1124,18 +1118,18 @@
         <v>0.80471895621705025</v>
       </c>
       <c r="L14" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="M14">
         <v>0</v>
       </c>
       <c r="N14" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B15">
         <v>4.6479999999999997E-9</v>
@@ -1144,7 +1138,7 @@
         <v>7</v>
       </c>
       <c r="E15" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F15" t="s">
         <v>19</v>
@@ -1173,18 +1167,18 @@
         <v>1.0397207708399181</v>
       </c>
       <c r="L15" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="M15">
         <v>0</v>
       </c>
       <c r="N15" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B16">
         <v>7.0301000000000005E-7</v>
@@ -1193,7 +1187,7 @@
         <v>7</v>
       </c>
       <c r="E16" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F16" t="s">
         <v>19</v>
@@ -1222,18 +1216,18 @@
         <v>1.0397207708399181</v>
       </c>
       <c r="L16" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="M16">
         <v>0</v>
       </c>
       <c r="N16" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B17">
         <v>5.3800599999999993E-9</v>
@@ -1242,7 +1236,7 @@
         <v>7</v>
       </c>
       <c r="E17" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F17" t="s">
         <v>19</v>
@@ -1271,18 +1265,18 @@
         <v>0.80471895621705025</v>
       </c>
       <c r="L17" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="M17">
         <v>0</v>
       </c>
       <c r="N17" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B18">
         <v>3.0734899999999997E-12</v>
@@ -1291,7 +1285,7 @@
         <v>7</v>
       </c>
       <c r="E18" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F18" t="s">
         <v>19</v>
@@ -1320,18 +1314,18 @@
         <v>0.80471895621705025</v>
       </c>
       <c r="L18" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="M18">
         <v>0</v>
       </c>
       <c r="N18" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B19">
         <v>5.3800599999999993E-6</v>
@@ -1340,7 +1334,7 @@
         <v>7</v>
       </c>
       <c r="E19" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F19" t="s">
         <v>19</v>
@@ -1359,13 +1353,13 @@
         <v>0.80471895621705025</v>
       </c>
       <c r="L19" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="M19">
         <v>0</v>
       </c>
       <c r="N19" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
@@ -1380,7 +1374,7 @@
         <v>7</v>
       </c>
       <c r="E20" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F20" t="s">
         <v>19</v>
@@ -1399,13 +1393,13 @@
         <v>2.439508208471609E-2</v>
       </c>
       <c r="L20" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="M20">
         <v>0</v>
       </c>
       <c r="N20" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
@@ -1419,7 +1413,7 @@
         <v>7</v>
       </c>
       <c r="E21" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F21" t="s">
         <v>19</v>
@@ -1438,18 +1432,18 @@
         <v>0.20273255405408211</v>
       </c>
       <c r="L21" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="M21">
         <v>0</v>
       </c>
       <c r="N21" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B22">
         <v>5.8099999999999994E-6</v>
@@ -1458,7 +1452,7 @@
         <v>7</v>
       </c>
       <c r="E22" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F22" t="s">
         <v>19</v>
@@ -1477,18 +1471,18 @@
         <v>0.54930614433405478</v>
       </c>
       <c r="L22" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="M22">
         <v>0</v>
       </c>
       <c r="N22" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B23">
         <v>1.6849E-16</v>
@@ -1497,7 +1491,7 @@
         <v>7</v>
       </c>
       <c r="E23" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F23" t="s">
         <v>19</v>
@@ -1516,18 +1510,18 @@
         <v>1.0397207708399181</v>
       </c>
       <c r="L23" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="M23">
         <v>0</v>
       </c>
       <c r="N23" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B24">
         <v>7.9596999999999994E-6</v>
@@ -1536,7 +1530,7 @@
         <v>7</v>
       </c>
       <c r="E24" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F24" t="s">
         <v>19</v>
@@ -1555,18 +1549,18 @@
         <v>0.80471895621705025</v>
       </c>
       <c r="L24" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="M24">
         <v>0</v>
       </c>
       <c r="N24" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B25">
         <v>1.9231099999999998E-7</v>
@@ -1575,7 +1569,7 @@
         <v>7</v>
       </c>
       <c r="E25" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F25" t="s">
         <v>19</v>
@@ -1594,18 +1588,18 @@
         <v>0.80471895621705025</v>
       </c>
       <c r="L25" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="M25">
         <v>0</v>
       </c>
       <c r="N25" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B26">
         <v>3.0502500000000001</v>
@@ -1614,7 +1608,7 @@
         <v>70</v>
       </c>
       <c r="E26" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F26" t="s">
         <v>19</v>
@@ -1633,18 +1627,18 @@
         <v>2.439508208471609E-2</v>
       </c>
       <c r="L26" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="M26">
         <v>0</v>
       </c>
       <c r="N26" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B27">
         <v>4.6073299999999995E-6</v>
@@ -1653,7 +1647,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F27" t="s">
         <v>19</v>
@@ -1672,18 +1666,18 @@
         <v>0.80471895621705025</v>
       </c>
       <c r="L27" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="M27">
         <v>0</v>
       </c>
       <c r="N27" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B28">
         <v>1.7429999999999998E-10</v>
@@ -1692,7 +1686,7 @@
         <v>7</v>
       </c>
       <c r="E28" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F28" t="s">
         <v>19</v>
@@ -1711,13 +1705,13 @@
         <v>0.80471895621705025</v>
       </c>
       <c r="L28" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="M28">
         <v>0</v>
       </c>
       <c r="N28" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
@@ -1731,7 +1725,7 @@
         <v>7</v>
       </c>
       <c r="E29" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F29" t="s">
         <v>19</v>
@@ -1750,13 +1744,13 @@
         <v>0.80471895621705025</v>
       </c>
       <c r="L29" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="M29">
         <v>0</v>
       </c>
       <c r="N29" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.2">
@@ -1770,7 +1764,7 @@
         <v>7</v>
       </c>
       <c r="E30" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F30" t="s">
         <v>19</v>
@@ -1789,18 +1783,18 @@
         <v>0.20273255405408211</v>
       </c>
       <c r="L30" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="M30">
         <v>0</v>
       </c>
       <c r="N30" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B31">
         <v>4.6479999999999997E-8</v>
@@ -1809,7 +1803,7 @@
         <v>7</v>
       </c>
       <c r="E31" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F31" t="s">
         <v>19</v>
@@ -1828,13 +1822,13 @@
         <v>1.0397207708399181</v>
       </c>
       <c r="L31" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="M31">
         <v>0</v>
       </c>
       <c r="N31" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
@@ -1848,7 +1842,7 @@
         <v>7</v>
       </c>
       <c r="E32" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F32" t="s">
         <v>19</v>
@@ -1867,18 +1861,18 @@
         <v>0.54930614433405478</v>
       </c>
       <c r="L32" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="M32">
         <v>0</v>
       </c>
       <c r="N32" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B33">
         <v>6.6814999999999995E-6</v>
@@ -1887,7 +1881,7 @@
         <v>7</v>
       </c>
       <c r="E33" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F33" t="s">
         <v>19</v>
@@ -1906,18 +1900,18 @@
         <v>0.80471895621705025</v>
       </c>
       <c r="L33" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="M33">
         <v>0</v>
       </c>
       <c r="N33" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B34">
         <v>4.0960499999999995E-6</v>
@@ -1926,7 +1920,7 @@
         <v>7</v>
       </c>
       <c r="E34" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F34" t="s">
         <v>19</v>
@@ -1945,18 +1939,18 @@
         <v>0.80471895621705025</v>
       </c>
       <c r="L34" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="M34">
         <v>0</v>
       </c>
       <c r="N34" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B35">
         <v>9.2959999999999993E-8</v>
@@ -1965,7 +1959,7 @@
         <v>7</v>
       </c>
       <c r="E35" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F35" t="s">
         <v>19</v>
@@ -1984,13 +1978,13 @@
         <v>1.0397207708399181</v>
       </c>
       <c r="L35" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="M35">
         <v>0</v>
       </c>
       <c r="N35" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.2">
@@ -2004,7 +1998,7 @@
         <v>7</v>
       </c>
       <c r="E36" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F36" t="s">
         <v>19</v>
@@ -2023,18 +2017,18 @@
         <v>4.7655089902162509E-2</v>
       </c>
       <c r="L36" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="M36">
         <v>0</v>
       </c>
       <c r="N36" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B37">
         <v>8.714999999999999E-9</v>
@@ -2043,7 +2037,7 @@
         <v>7</v>
       </c>
       <c r="E37" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F37" t="s">
         <v>19</v>
@@ -2062,18 +2056,18 @@
         <v>0.80471895621705025</v>
       </c>
       <c r="L37" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="M37">
         <v>0</v>
       </c>
       <c r="N37" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B38">
         <v>1.27239E-11</v>
@@ -2085,7 +2079,7 @@
         <v>6</v>
       </c>
       <c r="E38" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F38" t="s">
         <v>35</v>
@@ -2114,18 +2108,18 @@
         <v>0.3465735902799727</v>
       </c>
       <c r="L38" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="M38">
         <v>0</v>
       </c>
       <c r="N38" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B39">
         <v>1.4525000000000001E-5</v>
@@ -2137,7 +2131,7 @@
         <v>7</v>
       </c>
       <c r="E39" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F39" t="s">
         <v>35</v>
@@ -2156,18 +2150,18 @@
         <v>0.1075556898084728</v>
       </c>
       <c r="L39" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="M39">
         <v>0</v>
       </c>
       <c r="N39" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B40">
         <v>1.1619999999999999E-5</v>
@@ -2179,7 +2173,7 @@
         <v>7</v>
       </c>
       <c r="E40" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F40" t="s">
         <v>35</v>
@@ -2198,30 +2192,30 @@
         <v>0.1075556898084728</v>
       </c>
       <c r="L40" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="M40">
         <v>0</v>
       </c>
       <c r="N40" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B41">
         <v>2.9049999999999998</v>
       </c>
       <c r="C41" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D41" t="s">
         <v>7</v>
       </c>
       <c r="E41" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F41" t="s">
         <v>35</v>
@@ -2240,18 +2234,18 @@
         <v>0.45814536593707761</v>
       </c>
       <c r="L41" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="M41">
         <v>0</v>
       </c>
       <c r="N41" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B42">
         <f>(3.6/47.5)/0.62</f>
@@ -2264,7 +2258,7 @@
         <v>7</v>
       </c>
       <c r="E42" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F42" t="s">
         <v>35</v>
@@ -2283,18 +2277,18 @@
         <v>0</v>
       </c>
       <c r="L42" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="M42">
         <v>0</v>
       </c>
       <c r="N42" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B43">
         <v>-5.8099999999999994E-6</v>
@@ -2306,7 +2300,7 @@
         <v>7</v>
       </c>
       <c r="E43" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F43" t="s">
         <v>35</v>
@@ -2335,18 +2329,18 @@
         <v>1.0397207708399181</v>
       </c>
       <c r="L43" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="M43">
         <v>0</v>
       </c>
       <c r="N43" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.2">
       <c r="M44" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="45" spans="1:14" ht="16" x14ac:dyDescent="0.2">
@@ -2469,7 +2463,7 @@
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B56">
         <v>1.02</v>
@@ -2487,7 +2481,7 @@
         <v>35</v>
       </c>
       <c r="H56" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="57" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -2516,7 +2510,7 @@
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B58">
         <f>0.061874*0.669</f>
@@ -2535,7 +2529,7 @@
         <v>35</v>
       </c>
       <c r="H58" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
@@ -2674,7 +2668,7 @@
         <v>0</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.2">
@@ -2682,7 +2676,7 @@
         <v>1</v>
       </c>
       <c r="B67" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.2">
@@ -2706,7 +2700,7 @@
         <v>5</v>
       </c>
       <c r="B70" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.2">
@@ -2906,9 +2900,9 @@
         <v>28</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B81">
         <v>1</v>
@@ -2932,7 +2926,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>32</v>
       </c>
@@ -2961,7 +2955,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>39</v>
       </c>
@@ -2990,7 +2984,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>42</v>
       </c>
@@ -3019,7 +3013,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>46</v>
       </c>
@@ -3048,7 +3042,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>49</v>
       </c>
@@ -3071,7 +3065,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>51</v>
       </c>
@@ -3103,7 +3097,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>57</v>
       </c>
@@ -3132,7 +3126,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>61</v>
       </c>
@@ -3155,174 +3149,180 @@
         <v>63</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A90" t="s">
-        <v>96</v>
-      </c>
-      <c r="B90">
-        <v>55.5</v>
-      </c>
-      <c r="C90" t="s">
-        <v>17</v>
-      </c>
-      <c r="E90" t="s">
+    <row r="91" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="A91" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="92" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>64</v>
+      </c>
+      <c r="B92" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="93" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>2</v>
+      </c>
+      <c r="B93" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="94" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>4</v>
+      </c>
+      <c r="B94">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>5</v>
+      </c>
+      <c r="B95" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="96" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>6</v>
+      </c>
+      <c r="B96" t="s">
+        <v>7</v>
+      </c>
+      <c r="M96" s="2"/>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>66</v>
+      </c>
+      <c r="B97" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>79</v>
+      </c>
+      <c r="B98" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A99" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>9</v>
+      </c>
+      <c r="B100" t="s">
+        <v>10</v>
+      </c>
+      <c r="C100" t="s">
+        <v>11</v>
+      </c>
+      <c r="D100" t="s">
+        <v>2</v>
+      </c>
+      <c r="E100" t="s">
+        <v>6</v>
+      </c>
+      <c r="F100" t="s">
+        <v>13</v>
+      </c>
+      <c r="G100" t="s">
+        <v>67</v>
+      </c>
+      <c r="H100" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>57</v>
+      </c>
+      <c r="B101">
+        <v>1</v>
+      </c>
+      <c r="C101" t="s">
+        <v>29</v>
+      </c>
+      <c r="D101" t="s">
+        <v>58</v>
+      </c>
+      <c r="E101" t="s">
+        <v>7</v>
+      </c>
+      <c r="F101" t="s">
+        <v>30</v>
+      </c>
+      <c r="H101" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>68</v>
+      </c>
+      <c r="B102">
+        <v>2.3800000000000001E-4</v>
+      </c>
+      <c r="C102" t="s">
+        <v>33</v>
+      </c>
+      <c r="D102" t="s">
+        <v>69</v>
+      </c>
+      <c r="E102" t="s">
         <v>70</v>
       </c>
-      <c r="F90" t="s">
-        <v>97</v>
-      </c>
-      <c r="G90" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="92" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A92" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B92" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A93" t="s">
-        <v>64</v>
-      </c>
-      <c r="B93" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A94" t="s">
-        <v>2</v>
-      </c>
-      <c r="B94" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A95" t="s">
-        <v>4</v>
-      </c>
-      <c r="B95">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A96" t="s">
-        <v>5</v>
-      </c>
-      <c r="B96" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A97" t="s">
-        <v>6</v>
-      </c>
-      <c r="B97" t="s">
-        <v>7</v>
-      </c>
-      <c r="M97" s="2"/>
-    </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A98" t="s">
-        <v>66</v>
-      </c>
-      <c r="B98" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A99" t="s">
-        <v>79</v>
-      </c>
-      <c r="B99" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="100" spans="1:13" ht="16" x14ac:dyDescent="0.2">
-      <c r="A100" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A101" t="s">
-        <v>9</v>
-      </c>
-      <c r="B101" t="s">
-        <v>10</v>
-      </c>
-      <c r="C101" t="s">
-        <v>11</v>
-      </c>
-      <c r="D101" t="s">
-        <v>2</v>
-      </c>
-      <c r="E101" t="s">
-        <v>6</v>
-      </c>
-      <c r="F101" t="s">
-        <v>13</v>
-      </c>
-      <c r="G101" t="s">
-        <v>67</v>
-      </c>
-      <c r="H101" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A102" t="s">
-        <v>57</v>
-      </c>
-      <c r="B102">
-        <v>1</v>
-      </c>
-      <c r="C102" t="s">
-        <v>29</v>
-      </c>
-      <c r="D102" t="s">
-        <v>58</v>
-      </c>
-      <c r="E102" t="s">
-        <v>7</v>
-      </c>
       <c r="F102" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="H102" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.2">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="B103">
-        <v>2.3800000000000001E-4</v>
+        <v>3.4339655648031599E-10</v>
       </c>
       <c r="C103" t="s">
         <v>33</v>
       </c>
       <c r="D103" t="s">
-        <v>69</v>
+        <v>34</v>
       </c>
       <c r="E103" t="s">
-        <v>70</v>
+        <v>7</v>
       </c>
       <c r="F103" t="s">
         <v>35</v>
       </c>
+      <c r="G103" t="s">
+        <v>73</v>
+      </c>
       <c r="H103" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="104" spans="1:13" x14ac:dyDescent="0.2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="B104">
-        <v>3.4339655648031599E-10</v>
+        <v>1.8660000000000003E-2</v>
       </c>
       <c r="C104" t="s">
         <v>33</v>
@@ -3336,19 +3336,16 @@
       <c r="F104" t="s">
         <v>35</v>
       </c>
-      <c r="G104" t="s">
-        <v>73</v>
-      </c>
       <c r="H104" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="105" spans="1:13" x14ac:dyDescent="0.2">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B105">
-        <v>1.8660000000000003E-2</v>
+        <v>8.1000000000000013E-3</v>
       </c>
       <c r="C105" t="s">
         <v>33</v>
@@ -3363,21 +3360,21 @@
         <v>35</v>
       </c>
       <c r="H105" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="106" spans="1:13" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>77</v>
+        <v>49</v>
       </c>
       <c r="B106">
-        <v>8.1000000000000013E-3</v>
+        <v>0.996</v>
       </c>
       <c r="C106" t="s">
         <v>33</v>
       </c>
       <c r="D106" t="s">
-        <v>34</v>
+        <v>69</v>
       </c>
       <c r="E106" t="s">
         <v>7</v>
@@ -3386,52 +3383,29 @@
         <v>35</v>
       </c>
       <c r="H106" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="107" spans="1:13" x14ac:dyDescent="0.2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B107">
-        <v>0.996</v>
+        <v>3.44E-2</v>
       </c>
       <c r="C107" t="s">
         <v>33</v>
       </c>
       <c r="D107" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="E107" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="F107" t="s">
         <v>35</v>
       </c>
       <c r="H107" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="108" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A108" t="s">
-        <v>51</v>
-      </c>
-      <c r="B108">
-        <v>3.44E-2</v>
-      </c>
-      <c r="C108" t="s">
-        <v>33</v>
-      </c>
-      <c r="D108" t="s">
-        <v>58</v>
-      </c>
-      <c r="E108" t="s">
-        <v>52</v>
-      </c>
-      <c r="F108" t="s">
-        <v>35</v>
-      </c>
-      <c r="H108" t="s">
         <v>55</v>
       </c>
     </row>

</xml_diff>